<commit_message>
OrologioWEBPonto - Diagrama de casos de uso Diagrama De Classe OrologioWEBPonto
</commit_message>
<xml_diff>
--- a/Requisitos e Casos de Uso.xlsx
+++ b/Requisitos e Casos de Uso.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21840" windowHeight="9735"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21840" windowHeight="9735" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Plan1" sheetId="1" r:id="rId1"/>
+    <sheet name="CASOS DE USO" sheetId="1" r:id="rId1"/>
+    <sheet name="REQUISITOS DO SISTEMA" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="145621" concurrentCalc="0"/>
   <extLst>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="68">
   <si>
     <t>REQUISITOS DO SISTEMA</t>
   </si>
@@ -72,9 +73,6 @@
     <t>RE09</t>
   </si>
   <si>
-    <t>Manter registros de horários para cada funcionário agrupados por dia, quando houver registro</t>
-  </si>
-  <si>
     <t>Permitir ao usuário RH a alteração de dados cadastrais dos usuários funcionários</t>
   </si>
   <si>
@@ -204,16 +202,28 @@
     <t>UC13</t>
   </si>
   <si>
-    <t>UC14</t>
-  </si>
-  <si>
-    <t>MANTER REGISTRO</t>
-  </si>
-  <si>
-    <t>SISTEMA</t>
-  </si>
-  <si>
     <t>Cadastrar usuário administrador definindo(nome,login,senha,nivel,email)</t>
+  </si>
+  <si>
+    <t>RE13</t>
+  </si>
+  <si>
+    <t>RE14</t>
+  </si>
+  <si>
+    <t>RE15</t>
+  </si>
+  <si>
+    <t>Listar usuários cadastrados no sistema</t>
+  </si>
+  <si>
+    <t>Listar empresas cadastradas no sistema</t>
+  </si>
+  <si>
+    <t>Listar funcionários cadastrados no sistema</t>
+  </si>
+  <si>
+    <t>Permitir ao usuário administrador alterar o cadastro de empresas</t>
   </si>
 </sst>
 </file>
@@ -404,7 +414,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -413,6 +423,48 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -423,52 +475,13 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -742,7 +755,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -750,327 +763,399 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K16"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3:G16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="76.5703125" customWidth="1"/>
-    <col min="3" max="3" width="20" customWidth="1"/>
-    <col min="4" max="4" width="24" customWidth="1"/>
-    <col min="6" max="6" width="41.5703125" customWidth="1"/>
-    <col min="7" max="7" width="28.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="41.5703125" customWidth="1"/>
+    <col min="3" max="3" width="28.5703125" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" s="19"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="B8" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="C8" s="14" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B9" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="C9" s="14" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="B10" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="C10" s="14" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="B11" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="C11" s="14" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="B12" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="C12" s="14" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="B13" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="C13" s="14" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="B14" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="C14" s="14" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="B15" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="C15" s="17" t="s">
+        <v>43</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:C1"/>
+  </mergeCells>
+  <printOptions horizontalCentered="1"/>
+  <pageMargins left="0.51181102362204722" right="0.51181102362204722" top="0.78740157480314965" bottom="0.78740157480314965" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.5703125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="76.5703125" customWidth="1"/>
+    <col min="3" max="3" width="9.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="6"/>
-      <c r="E1" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="F1" s="5"/>
-      <c r="G1" s="17"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
+      <c r="B1" s="19"/>
+      <c r="C1" s="12"/>
+    </row>
+    <row r="2" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="E2" s="7" t="s">
+      <c r="C2" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="F2" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="G2" s="9" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="10" t="s">
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="C4" s="9" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="E3" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="F3" s="18" t="s">
-        <v>32</v>
-      </c>
-      <c r="G3" s="19" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="E4" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="F4" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="G4" s="19" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="12" t="s">
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C14" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="E5" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="F5" s="18" t="s">
-        <v>34</v>
-      </c>
-      <c r="G5" s="19" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="E6" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="F6" s="18" t="s">
-        <v>31</v>
-      </c>
-      <c r="G6" s="19" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="C7" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="E7" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="F7" s="18" t="s">
-        <v>35</v>
-      </c>
-      <c r="G7" s="19" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="C8" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="E8" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="F8" s="18" t="s">
-        <v>36</v>
-      </c>
-      <c r="G8" s="19" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="B9" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="C9" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="E9" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="F9" s="18" t="s">
-        <v>37</v>
-      </c>
-      <c r="G9" s="19" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="B10" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="C10" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="E10" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="F10" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="G10" s="19" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="B11" s="11" t="s">
+    </row>
+    <row r="15" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A16" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="B17" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="E11" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="F11" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="G11" s="19" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="B12" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="C12" s="12" t="s">
+      <c r="C17" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="E12" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="F12" s="18" t="s">
-        <v>40</v>
-      </c>
-      <c r="G12" s="19" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="A13" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="B13" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="C13" s="12" t="s">
-        <v>60</v>
-      </c>
-      <c r="E13" s="10" t="s">
-        <v>58</v>
-      </c>
-      <c r="F13" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="G13" s="19" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="B14" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="C14" s="16" t="s">
-        <v>61</v>
-      </c>
-      <c r="E14" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="F14" s="18" t="s">
-        <v>62</v>
-      </c>
-      <c r="G14" s="19" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C15" s="2"/>
-      <c r="E15" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="F15" s="18" t="s">
-        <v>42</v>
-      </c>
-      <c r="G15" s="19" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E16" s="20" t="s">
-        <v>61</v>
-      </c>
-      <c r="F16" s="21" t="s">
-        <v>43</v>
-      </c>
-      <c r="G16" s="22" t="s">
-        <v>44</v>
-      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C18" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="1">
     <mergeCell ref="A1:B1"/>
-    <mergeCell ref="E1:G1"/>
   </mergeCells>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>